<commit_message>
Changed excel cell property from "Standard" to "Text"
Otherwise numbers beginning with leading zero could be capped.

Example:
012345 will be transformed in excel to 12345
</commit_message>
<xml_diff>
--- a/Vorlage_Telefonbuch.xlsx
+++ b/Vorlage_Telefonbuch.xlsx
@@ -532,8 +532,9 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20 % - Akzent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -858,40 +859,43 @@
   <dimension ref="A1:J1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="A2:C2"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="16384" width="11.42578125" style="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>